<commit_message>
Added loggers in test classes and checking of alert
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/output/CandidateDetails.xlsx
+++ b/src/test/resources/testdata/output/CandidateDetails.xlsx
@@ -26,16 +26,16 @@
     <t>Result</t>
   </si>
   <si>
-    <t>failureResult</t>
+    <t>failureReason</t>
   </si>
   <si>
-    <t>CTX678883</t>
+    <t>CTX456161</t>
   </si>
   <si>
-    <t xml:space="preserve"> Michael</t>
+    <t xml:space="preserve"> Rajesh</t>
   </si>
   <si>
-    <t>Gutierrez Chávez</t>
+    <t>Shankar</t>
   </si>
   <si>
     <t>Don't Apply Inbound Record to Master Record</t>

</xml_diff>